<commit_message>
ordinary and DatabaseUtil.close()をfinally blockに
</commit_message>
<xml_diff>
--- a/document/expr10/model_config.xlsx
+++ b/document/expr10/model_config.xlsx
@@ -2067,7 +2067,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6680" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6699" uniqueCount="594">
   <si>
     <t>no</t>
     <phoneticPr fontId="4"/>
@@ -9778,6 +9778,190 @@
   </si>
   <si>
     <t>90</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>20221101</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>20221105</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>arff_3</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>clf_3</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>'ip', 'G3', 'G2'</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <r>
+      <t># wk1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> B1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>인것만</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>학습해본다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. ip,G3,G2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>대상</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  -&gt; python BoatLGBMClassifierTest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>실행해보니</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> precision</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>낮아서</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>포기</t>
+    </r>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -10022,7 +10206,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10214,6 +10398,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -13079,16 +13266,16 @@
   <sheetPr filterMode="1">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:V284"/>
+  <dimension ref="A1:V286"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T181" sqref="T181:T184"/>
+      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D186" sqref="D186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="9" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="9" customWidth="1"/>
     <col min="2" max="2" width="9.75" style="3" customWidth="1"/>
     <col min="3" max="3" width="10" style="3" customWidth="1"/>
     <col min="4" max="4" width="16.125" style="3" customWidth="1"/>
@@ -20788,10 +20975,10 @@
         <v>99100</v>
       </c>
       <c r="B165" s="121" t="s">
-        <v>580</v>
+        <v>588</v>
       </c>
       <c r="C165" s="121" t="s">
-        <v>583</v>
+        <v>589</v>
       </c>
       <c r="D165" s="117" t="s">
         <v>23</v>
@@ -20850,10 +21037,10 @@
         <v>99080</v>
       </c>
       <c r="B166" s="121" t="s">
-        <v>580</v>
+        <v>588</v>
       </c>
       <c r="C166" s="121" t="s">
-        <v>583</v>
+        <v>589</v>
       </c>
       <c r="D166" s="117" t="s">
         <v>23</v>
@@ -20912,10 +21099,10 @@
         <v>99083</v>
       </c>
       <c r="B167" s="121" t="s">
-        <v>580</v>
+        <v>588</v>
       </c>
       <c r="C167" s="121" t="s">
-        <v>583</v>
+        <v>589</v>
       </c>
       <c r="D167" s="117" t="s">
         <v>23</v>
@@ -20974,10 +21161,10 @@
         <v>99102</v>
       </c>
       <c r="B168" s="121" t="s">
-        <v>580</v>
+        <v>588</v>
       </c>
       <c r="C168" s="121" t="s">
-        <v>583</v>
+        <v>589</v>
       </c>
       <c r="D168" s="53" t="s">
         <v>119</v>
@@ -21036,10 +21223,10 @@
         <v>99103</v>
       </c>
       <c r="B169" s="121" t="s">
-        <v>580</v>
+        <v>588</v>
       </c>
       <c r="C169" s="121" t="s">
-        <v>583</v>
+        <v>589</v>
       </c>
       <c r="D169" s="53" t="s">
         <v>245</v>
@@ -21910,7 +22097,9 @@
       </c>
     </row>
     <row r="185" spans="1:20" s="119" customFormat="1">
-      <c r="A185" s="121"/>
+      <c r="A185" s="121" t="s">
+        <v>593</v>
+      </c>
       <c r="B185" s="121"/>
       <c r="C185" s="121"/>
       <c r="D185" s="53"/>
@@ -21932,59 +22121,93 @@
       <c r="T185" s="117"/>
     </row>
     <row r="186" spans="1:20" s="119" customFormat="1">
-      <c r="A186" s="134" t="s">
+      <c r="A186" s="135">
+        <v>96100</v>
+      </c>
+      <c r="B186" s="121" t="s">
+        <v>71</v>
+      </c>
+      <c r="C186" s="121" t="s">
+        <v>583</v>
+      </c>
+      <c r="D186" s="117" t="s">
+        <v>23</v>
+      </c>
+      <c r="E186" s="121" t="s">
+        <v>110</v>
+      </c>
+      <c r="F186" s="121" t="s">
+        <v>111</v>
+      </c>
+      <c r="G186" s="117" t="s">
+        <v>35</v>
+      </c>
+      <c r="H186" s="117" t="s">
+        <v>35</v>
+      </c>
+      <c r="I186" s="117" t="s">
+        <v>35</v>
+      </c>
+      <c r="J186" s="121" t="s">
+        <v>431</v>
+      </c>
+      <c r="K186" s="121" t="s">
+        <v>431</v>
+      </c>
+      <c r="L186" s="121" t="s">
+        <v>431</v>
+      </c>
+      <c r="M186" s="117" t="s">
+        <v>590</v>
+      </c>
+      <c r="N186" s="117" t="s">
+        <v>591</v>
+      </c>
+      <c r="O186" s="120" t="s">
+        <v>592</v>
+      </c>
+      <c r="P186" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q186" s="117" t="s">
+        <v>0</v>
+      </c>
+      <c r="R186" s="117" t="s">
+        <v>1</v>
+      </c>
+      <c r="S186" s="117">
+        <v>1825</v>
+      </c>
+      <c r="T186" s="117" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="187" spans="1:20" s="119" customFormat="1">
+      <c r="A187" s="121"/>
+      <c r="B187" s="121"/>
+      <c r="C187" s="121"/>
+      <c r="D187" s="53"/>
+      <c r="E187" s="117"/>
+      <c r="F187" s="117"/>
+      <c r="G187" s="117"/>
+      <c r="H187" s="117"/>
+      <c r="I187" s="117"/>
+      <c r="J187" s="121"/>
+      <c r="K187" s="117"/>
+      <c r="L187" s="117"/>
+      <c r="M187" s="117"/>
+      <c r="N187" s="117"/>
+      <c r="O187" s="120"/>
+      <c r="P187" s="117"/>
+      <c r="Q187" s="117"/>
+      <c r="R187" s="117"/>
+      <c r="S187" s="117"/>
+      <c r="T187" s="117"/>
+    </row>
+    <row r="188" spans="1:20" s="119" customFormat="1">
+      <c r="A188" s="134" t="s">
         <v>560</v>
       </c>
-      <c r="B186" s="121"/>
-      <c r="C186" s="121"/>
-      <c r="D186" s="121"/>
-      <c r="E186" s="121"/>
-      <c r="F186" s="121"/>
-      <c r="G186" s="121"/>
-      <c r="H186" s="121"/>
-      <c r="I186" s="121"/>
-      <c r="J186" s="121"/>
-      <c r="K186" s="121"/>
-      <c r="L186" s="121"/>
-      <c r="M186" s="121"/>
-      <c r="N186" s="121"/>
-      <c r="O186" s="121"/>
-      <c r="P186" s="121"/>
-      <c r="Q186" s="121"/>
-      <c r="R186" s="121"/>
-      <c r="S186" s="121"/>
-      <c r="T186" s="121"/>
-    </row>
-    <row r="187" spans="1:20" s="119" customFormat="1">
-      <c r="A187" s="123" t="s">
-        <v>559</v>
-      </c>
-      <c r="B187" s="121" t="s">
-        <v>71</v>
-      </c>
-      <c r="C187" s="121" t="s">
-        <v>554</v>
-      </c>
-      <c r="D187" s="121"/>
-      <c r="E187" s="121"/>
-      <c r="F187" s="121"/>
-      <c r="G187" s="121"/>
-      <c r="H187" s="121"/>
-      <c r="I187" s="121"/>
-      <c r="J187" s="121"/>
-      <c r="K187" s="121"/>
-      <c r="L187" s="121"/>
-      <c r="M187" s="121"/>
-      <c r="N187" s="121"/>
-      <c r="O187" s="121"/>
-      <c r="P187" s="121"/>
-      <c r="Q187" s="121"/>
-      <c r="R187" s="121"/>
-      <c r="S187" s="121"/>
-      <c r="T187" s="121"/>
-    </row>
-    <row r="188" spans="1:20" s="119" customFormat="1">
-      <c r="A188" s="123"/>
       <c r="B188" s="121"/>
       <c r="C188" s="121"/>
       <c r="D188" s="121"/>
@@ -22006,9 +22229,15 @@
       <c r="T188" s="121"/>
     </row>
     <row r="189" spans="1:20" s="119" customFormat="1">
-      <c r="A189" s="123"/>
-      <c r="B189" s="121"/>
-      <c r="C189" s="121"/>
+      <c r="A189" s="123" t="s">
+        <v>559</v>
+      </c>
+      <c r="B189" s="121" t="s">
+        <v>71</v>
+      </c>
+      <c r="C189" s="121" t="s">
+        <v>554</v>
+      </c>
       <c r="D189" s="121"/>
       <c r="E189" s="121"/>
       <c r="F189" s="121"/>
@@ -22049,7 +22278,7 @@
       <c r="S190" s="121"/>
       <c r="T190" s="121"/>
     </row>
-    <row r="191" spans="1:20">
+    <row r="191" spans="1:20" s="119" customFormat="1">
       <c r="A191" s="123"/>
       <c r="B191" s="121"/>
       <c r="C191" s="121"/>
@@ -22071,7 +22300,7 @@
       <c r="S191" s="121"/>
       <c r="T191" s="121"/>
     </row>
-    <row r="192" spans="1:20">
+    <row r="192" spans="1:20" s="119" customFormat="1">
       <c r="A192" s="123"/>
       <c r="B192" s="121"/>
       <c r="C192" s="121"/>
@@ -22093,7 +22322,7 @@
       <c r="S192" s="121"/>
       <c r="T192" s="121"/>
     </row>
-    <row r="193" spans="1:20" s="119" customFormat="1">
+    <row r="193" spans="1:20">
       <c r="A193" s="123"/>
       <c r="B193" s="121"/>
       <c r="C193" s="121"/>
@@ -22115,7 +22344,7 @@
       <c r="S193" s="121"/>
       <c r="T193" s="121"/>
     </row>
-    <row r="194" spans="1:20" s="77" customFormat="1">
+    <row r="194" spans="1:20">
       <c r="A194" s="123"/>
       <c r="B194" s="121"/>
       <c r="C194" s="121"/>
@@ -22159,223 +22388,143 @@
       <c r="S195" s="121"/>
       <c r="T195" s="121"/>
     </row>
-    <row r="196" spans="1:20" s="119" customFormat="1">
-      <c r="A196" s="9"/>
-      <c r="B196" s="3"/>
-      <c r="C196" s="3"/>
-      <c r="D196" s="3"/>
-      <c r="E196" s="3"/>
-      <c r="F196" s="3"/>
-      <c r="G196" s="3"/>
-      <c r="H196" s="3"/>
-      <c r="I196" s="3"/>
-      <c r="J196" s="3"/>
-      <c r="K196" s="3"/>
-      <c r="L196" s="3"/>
-      <c r="M196" s="3"/>
-      <c r="N196" s="3"/>
-      <c r="O196" s="3"/>
-      <c r="P196" s="3"/>
-      <c r="Q196" s="3"/>
-      <c r="R196" s="3"/>
-      <c r="S196" s="3"/>
-      <c r="T196" s="3"/>
+    <row r="196" spans="1:20" s="77" customFormat="1">
+      <c r="A196" s="123"/>
+      <c r="B196" s="121"/>
+      <c r="C196" s="121"/>
+      <c r="D196" s="121"/>
+      <c r="E196" s="121"/>
+      <c r="F196" s="121"/>
+      <c r="G196" s="121"/>
+      <c r="H196" s="121"/>
+      <c r="I196" s="121"/>
+      <c r="J196" s="121"/>
+      <c r="K196" s="121"/>
+      <c r="L196" s="121"/>
+      <c r="M196" s="121"/>
+      <c r="N196" s="121"/>
+      <c r="O196" s="121"/>
+      <c r="P196" s="121"/>
+      <c r="Q196" s="121"/>
+      <c r="R196" s="121"/>
+      <c r="S196" s="121"/>
+      <c r="T196" s="121"/>
     </row>
     <row r="197" spans="1:20" s="119" customFormat="1">
-      <c r="A197" s="9"/>
-      <c r="B197" s="3"/>
-      <c r="C197" s="3"/>
-      <c r="D197" s="3"/>
-      <c r="E197" s="3"/>
-      <c r="F197" s="3"/>
-      <c r="G197" s="3"/>
-      <c r="H197" s="3"/>
-      <c r="I197" s="3"/>
-      <c r="J197" s="3"/>
-      <c r="K197" s="3"/>
-      <c r="L197" s="3"/>
-      <c r="M197" s="3"/>
-      <c r="N197" s="3"/>
-      <c r="O197" s="3"/>
-      <c r="P197" s="3"/>
-      <c r="Q197" s="3"/>
-      <c r="R197" s="3"/>
-      <c r="S197" s="3"/>
-      <c r="T197" s="3"/>
+      <c r="A197" s="123"/>
+      <c r="B197" s="121"/>
+      <c r="C197" s="121"/>
+      <c r="D197" s="121"/>
+      <c r="E197" s="121"/>
+      <c r="F197" s="121"/>
+      <c r="G197" s="121"/>
+      <c r="H197" s="121"/>
+      <c r="I197" s="121"/>
+      <c r="J197" s="121"/>
+      <c r="K197" s="121"/>
+      <c r="L197" s="121"/>
+      <c r="M197" s="121"/>
+      <c r="N197" s="121"/>
+      <c r="O197" s="121"/>
+      <c r="P197" s="121"/>
+      <c r="Q197" s="121"/>
+      <c r="R197" s="121"/>
+      <c r="S197" s="121"/>
+      <c r="T197" s="121"/>
     </row>
     <row r="198" spans="1:20" s="119" customFormat="1">
-      <c r="A198" s="123"/>
-      <c r="B198" s="121"/>
-      <c r="C198" s="121"/>
-      <c r="D198" s="121"/>
-      <c r="E198" s="121"/>
-      <c r="F198" s="121"/>
-      <c r="G198" s="121"/>
-      <c r="H198" s="121"/>
-      <c r="I198" s="121"/>
-      <c r="J198" s="121"/>
-      <c r="K198" s="121"/>
-      <c r="L198" s="121"/>
-      <c r="M198" s="121"/>
-      <c r="N198" s="121"/>
-      <c r="O198" s="121"/>
-      <c r="P198" s="121"/>
-      <c r="Q198" s="121"/>
-      <c r="R198" s="121"/>
-      <c r="S198" s="121"/>
-      <c r="T198" s="121"/>
+      <c r="A198" s="9"/>
+      <c r="B198" s="3"/>
+      <c r="C198" s="3"/>
+      <c r="D198" s="3"/>
+      <c r="E198" s="3"/>
+      <c r="F198" s="3"/>
+      <c r="G198" s="3"/>
+      <c r="H198" s="3"/>
+      <c r="I198" s="3"/>
+      <c r="J198" s="3"/>
+      <c r="K198" s="3"/>
+      <c r="L198" s="3"/>
+      <c r="M198" s="3"/>
+      <c r="N198" s="3"/>
+      <c r="O198" s="3"/>
+      <c r="P198" s="3"/>
+      <c r="Q198" s="3"/>
+      <c r="R198" s="3"/>
+      <c r="S198" s="3"/>
+      <c r="T198" s="3"/>
     </row>
     <row r="199" spans="1:20" s="119" customFormat="1">
-      <c r="A199" s="130" t="s">
+      <c r="A199" s="9"/>
+      <c r="B199" s="3"/>
+      <c r="C199" s="3"/>
+      <c r="D199" s="3"/>
+      <c r="E199" s="3"/>
+      <c r="F199" s="3"/>
+      <c r="G199" s="3"/>
+      <c r="H199" s="3"/>
+      <c r="I199" s="3"/>
+      <c r="J199" s="3"/>
+      <c r="K199" s="3"/>
+      <c r="L199" s="3"/>
+      <c r="M199" s="3"/>
+      <c r="N199" s="3"/>
+      <c r="O199" s="3"/>
+      <c r="P199" s="3"/>
+      <c r="Q199" s="3"/>
+      <c r="R199" s="3"/>
+      <c r="S199" s="3"/>
+      <c r="T199" s="3"/>
+    </row>
+    <row r="200" spans="1:20" s="119" customFormat="1">
+      <c r="A200" s="123"/>
+      <c r="B200" s="121"/>
+      <c r="C200" s="121"/>
+      <c r="D200" s="121"/>
+      <c r="E200" s="121"/>
+      <c r="F200" s="121"/>
+      <c r="G200" s="121"/>
+      <c r="H200" s="121"/>
+      <c r="I200" s="121"/>
+      <c r="J200" s="121"/>
+      <c r="K200" s="121"/>
+      <c r="L200" s="121"/>
+      <c r="M200" s="121"/>
+      <c r="N200" s="121"/>
+      <c r="O200" s="121"/>
+      <c r="P200" s="121"/>
+      <c r="Q200" s="121"/>
+      <c r="R200" s="121"/>
+      <c r="S200" s="121"/>
+      <c r="T200" s="121"/>
+    </row>
+    <row r="201" spans="1:20" s="119" customFormat="1">
+      <c r="A201" s="130" t="s">
         <v>528</v>
       </c>
-      <c r="B199" s="80"/>
-      <c r="C199" s="80"/>
-      <c r="D199" s="80"/>
-      <c r="E199" s="80"/>
-      <c r="F199" s="80"/>
-      <c r="G199" s="121"/>
-      <c r="H199" s="121"/>
-      <c r="I199" s="121"/>
-      <c r="J199" s="121"/>
-      <c r="K199" s="121"/>
-      <c r="L199" s="121"/>
-      <c r="M199" s="121"/>
-      <c r="N199" s="80"/>
-      <c r="O199" s="80"/>
-      <c r="P199" s="80"/>
-      <c r="Q199" s="80"/>
-      <c r="R199" s="80"/>
-      <c r="S199" s="80"/>
-      <c r="T199" s="80"/>
-    </row>
-    <row r="200" spans="1:20" s="119" customFormat="1">
-      <c r="A200" s="8">
+      <c r="B201" s="80"/>
+      <c r="C201" s="80"/>
+      <c r="D201" s="80"/>
+      <c r="E201" s="80"/>
+      <c r="F201" s="80"/>
+      <c r="G201" s="121"/>
+      <c r="H201" s="121"/>
+      <c r="I201" s="121"/>
+      <c r="J201" s="121"/>
+      <c r="K201" s="121"/>
+      <c r="L201" s="121"/>
+      <c r="M201" s="121"/>
+      <c r="N201" s="80"/>
+      <c r="O201" s="80"/>
+      <c r="P201" s="80"/>
+      <c r="Q201" s="80"/>
+      <c r="R201" s="80"/>
+      <c r="S201" s="80"/>
+      <c r="T201" s="80"/>
+    </row>
+    <row r="202" spans="1:20" s="119" customFormat="1">
+      <c r="A202" s="8">
         <v>99069</v>
-      </c>
-      <c r="B200" s="121" t="s">
-        <v>71</v>
-      </c>
-      <c r="C200" s="121" t="s">
-        <v>55</v>
-      </c>
-      <c r="D200" s="121" t="s">
-        <v>23</v>
-      </c>
-      <c r="E200" s="121" t="s">
-        <v>110</v>
-      </c>
-      <c r="F200" s="121" t="s">
-        <v>111</v>
-      </c>
-      <c r="G200" s="117" t="s">
-        <v>34</v>
-      </c>
-      <c r="H200" s="117" t="s">
-        <v>34</v>
-      </c>
-      <c r="I200" s="117" t="s">
-        <v>34</v>
-      </c>
-      <c r="J200" s="121" t="s">
-        <v>431</v>
-      </c>
-      <c r="K200" s="121" t="s">
-        <v>431</v>
-      </c>
-      <c r="L200" s="121" t="s">
-        <v>431</v>
-      </c>
-      <c r="M200" s="117" t="s">
-        <v>22</v>
-      </c>
-      <c r="N200" s="117" t="s">
-        <v>47</v>
-      </c>
-      <c r="O200" s="120" t="s">
-        <v>48</v>
-      </c>
-      <c r="P200" s="117" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q200" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="R200" s="117" t="s">
-        <v>1</v>
-      </c>
-      <c r="S200" s="117">
-        <v>1825</v>
-      </c>
-      <c r="T200" s="117" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="201" spans="1:20" s="119" customFormat="1">
-      <c r="A201" s="8">
-        <v>99072</v>
-      </c>
-      <c r="B201" s="121" t="s">
-        <v>71</v>
-      </c>
-      <c r="C201" s="121" t="s">
-        <v>55</v>
-      </c>
-      <c r="D201" s="121" t="s">
-        <v>23</v>
-      </c>
-      <c r="E201" s="121" t="s">
-        <v>110</v>
-      </c>
-      <c r="F201" s="121" t="s">
-        <v>111</v>
-      </c>
-      <c r="G201" s="117" t="s">
-        <v>433</v>
-      </c>
-      <c r="H201" s="117" t="s">
-        <v>433</v>
-      </c>
-      <c r="I201" s="117" t="s">
-        <v>433</v>
-      </c>
-      <c r="J201" s="121" t="s">
-        <v>431</v>
-      </c>
-      <c r="K201" s="121" t="s">
-        <v>431</v>
-      </c>
-      <c r="L201" s="121" t="s">
-        <v>431</v>
-      </c>
-      <c r="M201" s="117" t="s">
-        <v>22</v>
-      </c>
-      <c r="N201" s="117" t="s">
-        <v>47</v>
-      </c>
-      <c r="O201" s="120" t="s">
-        <v>48</v>
-      </c>
-      <c r="P201" s="117" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q201" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="R201" s="117" t="s">
-        <v>1</v>
-      </c>
-      <c r="S201" s="117">
-        <v>1825</v>
-      </c>
-      <c r="T201" s="117" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="202" spans="1:20" s="119" customFormat="1">
-      <c r="A202" s="123">
-        <v>99081</v>
       </c>
       <c r="B202" s="121" t="s">
         <v>71</v>
@@ -22384,7 +22533,7 @@
         <v>55</v>
       </c>
       <c r="D202" s="121" t="s">
-        <v>440</v>
+        <v>23</v>
       </c>
       <c r="E202" s="121" t="s">
         <v>110</v>
@@ -22401,14 +22550,14 @@
       <c r="I202" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="J202" s="117" t="s">
-        <v>77</v>
-      </c>
-      <c r="K202" s="117" t="s">
-        <v>77</v>
-      </c>
-      <c r="L202" s="117" t="s">
-        <v>77</v>
+      <c r="J202" s="121" t="s">
+        <v>431</v>
+      </c>
+      <c r="K202" s="121" t="s">
+        <v>431</v>
+      </c>
+      <c r="L202" s="121" t="s">
+        <v>431</v>
       </c>
       <c r="M202" s="117" t="s">
         <v>22</v>
@@ -22436,8 +22585,8 @@
       </c>
     </row>
     <row r="203" spans="1:20" s="119" customFormat="1">
-      <c r="A203" s="123">
-        <v>99082</v>
+      <c r="A203" s="8">
+        <v>99072</v>
       </c>
       <c r="B203" s="121" t="s">
         <v>71</v>
@@ -22454,23 +22603,23 @@
       <c r="F203" s="121" t="s">
         <v>111</v>
       </c>
-      <c r="G203" s="119" t="s">
+      <c r="G203" s="117" t="s">
         <v>433</v>
       </c>
-      <c r="H203" s="119" t="s">
+      <c r="H203" s="117" t="s">
         <v>433</v>
       </c>
-      <c r="I203" s="119" t="s">
+      <c r="I203" s="117" t="s">
         <v>433</v>
       </c>
-      <c r="J203" s="117" t="s">
-        <v>77</v>
-      </c>
-      <c r="K203" s="117" t="s">
-        <v>77</v>
-      </c>
-      <c r="L203" s="117" t="s">
-        <v>77</v>
+      <c r="J203" s="121" t="s">
+        <v>431</v>
+      </c>
+      <c r="K203" s="121" t="s">
+        <v>431</v>
+      </c>
+      <c r="L203" s="121" t="s">
+        <v>431</v>
       </c>
       <c r="M203" s="117" t="s">
         <v>22</v>
@@ -22499,7 +22648,7 @@
     </row>
     <row r="204" spans="1:20" s="119" customFormat="1">
       <c r="A204" s="123">
-        <v>99084</v>
+        <v>99081</v>
       </c>
       <c r="B204" s="121" t="s">
         <v>71</v>
@@ -22508,7 +22657,7 @@
         <v>55</v>
       </c>
       <c r="D204" s="121" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E204" s="121" t="s">
         <v>110</v>
@@ -22526,13 +22675,13 @@
         <v>34</v>
       </c>
       <c r="J204" s="117" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K204" s="117" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L204" s="117" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M204" s="117" t="s">
         <v>22</v>
@@ -22561,7 +22710,7 @@
     </row>
     <row r="205" spans="1:20" s="119" customFormat="1">
       <c r="A205" s="123">
-        <v>99085</v>
+        <v>99082</v>
       </c>
       <c r="B205" s="121" t="s">
         <v>71</v>
@@ -22588,13 +22737,13 @@
         <v>433</v>
       </c>
       <c r="J205" s="117" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K205" s="117" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L205" s="117" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M205" s="117" t="s">
         <v>22</v>
@@ -22623,7 +22772,7 @@
     </row>
     <row r="206" spans="1:20" s="119" customFormat="1">
       <c r="A206" s="123">
-        <v>99087</v>
+        <v>99084</v>
       </c>
       <c r="B206" s="121" t="s">
         <v>71</v>
@@ -22632,7 +22781,7 @@
         <v>55</v>
       </c>
       <c r="D206" s="121" t="s">
-        <v>23</v>
+        <v>442</v>
       </c>
       <c r="E206" s="121" t="s">
         <v>110</v>
@@ -22650,13 +22799,13 @@
         <v>34</v>
       </c>
       <c r="J206" s="117" t="s">
-        <v>447</v>
+        <v>78</v>
       </c>
       <c r="K206" s="117" t="s">
-        <v>447</v>
+        <v>78</v>
       </c>
       <c r="L206" s="117" t="s">
-        <v>447</v>
+        <v>78</v>
       </c>
       <c r="M206" s="117" t="s">
         <v>22</v>
@@ -22683,9 +22832,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="207" spans="1:20">
+    <row r="207" spans="1:20" s="119" customFormat="1">
       <c r="A207" s="123">
-        <v>99088</v>
+        <v>99085</v>
       </c>
       <c r="B207" s="121" t="s">
         <v>71</v>
@@ -22712,13 +22861,13 @@
         <v>433</v>
       </c>
       <c r="J207" s="117" t="s">
-        <v>447</v>
+        <v>78</v>
       </c>
       <c r="K207" s="117" t="s">
-        <v>447</v>
+        <v>78</v>
       </c>
       <c r="L207" s="117" t="s">
-        <v>447</v>
+        <v>78</v>
       </c>
       <c r="M207" s="117" t="s">
         <v>22</v>
@@ -22745,9 +22894,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="208" spans="1:20">
+    <row r="208" spans="1:20" s="119" customFormat="1">
       <c r="A208" s="123">
-        <v>99090</v>
+        <v>99087</v>
       </c>
       <c r="B208" s="121" t="s">
         <v>71</v>
@@ -22774,13 +22923,13 @@
         <v>34</v>
       </c>
       <c r="J208" s="117" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K208" s="117" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L208" s="117" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="M208" s="117" t="s">
         <v>22</v>
@@ -22809,7 +22958,7 @@
     </row>
     <row r="209" spans="1:20">
       <c r="A209" s="123">
-        <v>99091</v>
+        <v>99088</v>
       </c>
       <c r="B209" s="121" t="s">
         <v>71</v>
@@ -22836,13 +22985,13 @@
         <v>433</v>
       </c>
       <c r="J209" s="117" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K209" s="117" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L209" s="117" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="M209" s="117" t="s">
         <v>22</v>
@@ -22871,7 +23020,7 @@
     </row>
     <row r="210" spans="1:20">
       <c r="A210" s="123">
-        <v>99095</v>
+        <v>99090</v>
       </c>
       <c r="B210" s="121" t="s">
         <v>71</v>
@@ -22898,13 +23047,13 @@
         <v>34</v>
       </c>
       <c r="J210" s="117" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K210" s="117" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="L210" s="117" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="M210" s="117" t="s">
         <v>22</v>
@@ -22933,7 +23082,7 @@
     </row>
     <row r="211" spans="1:20">
       <c r="A211" s="123">
-        <v>99096</v>
+        <v>99091</v>
       </c>
       <c r="B211" s="121" t="s">
         <v>71</v>
@@ -22960,13 +23109,13 @@
         <v>433</v>
       </c>
       <c r="J211" s="117" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K211" s="117" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="L211" s="117" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="M211" s="117" t="s">
         <v>22</v>
@@ -22993,49 +23142,129 @@
         <v>25</v>
       </c>
     </row>
-    <row r="216" spans="1:20" s="119" customFormat="1">
-      <c r="A216" s="9"/>
-      <c r="B216" s="3"/>
-      <c r="C216" s="3"/>
-      <c r="D216" s="3"/>
-      <c r="E216" s="3"/>
-      <c r="F216" s="3"/>
-      <c r="G216" s="3"/>
-      <c r="H216" s="3"/>
-      <c r="I216" s="3"/>
-      <c r="J216" s="3"/>
-      <c r="K216" s="3"/>
-      <c r="L216" s="3"/>
-      <c r="M216" s="3"/>
-      <c r="N216" s="3"/>
-      <c r="O216" s="3"/>
-      <c r="P216" s="3"/>
-      <c r="Q216" s="3"/>
-      <c r="R216" s="3"/>
-      <c r="S216" s="3"/>
-      <c r="T216" s="3"/>
-    </row>
-    <row r="217" spans="1:20" s="119" customFormat="1">
-      <c r="A217" s="9"/>
-      <c r="B217" s="3"/>
-      <c r="C217" s="3"/>
-      <c r="D217" s="3"/>
-      <c r="E217" s="3"/>
-      <c r="F217" s="3"/>
-      <c r="G217" s="3"/>
-      <c r="H217" s="3"/>
-      <c r="I217" s="3"/>
-      <c r="J217" s="3"/>
-      <c r="K217" s="3"/>
-      <c r="L217" s="3"/>
-      <c r="M217" s="3"/>
-      <c r="N217" s="3"/>
-      <c r="O217" s="3"/>
-      <c r="P217" s="3"/>
-      <c r="Q217" s="3"/>
-      <c r="R217" s="3"/>
-      <c r="S217" s="3"/>
-      <c r="T217" s="3"/>
+    <row r="212" spans="1:20">
+      <c r="A212" s="123">
+        <v>99095</v>
+      </c>
+      <c r="B212" s="121" t="s">
+        <v>71</v>
+      </c>
+      <c r="C212" s="121" t="s">
+        <v>55</v>
+      </c>
+      <c r="D212" s="121" t="s">
+        <v>23</v>
+      </c>
+      <c r="E212" s="121" t="s">
+        <v>110</v>
+      </c>
+      <c r="F212" s="121" t="s">
+        <v>111</v>
+      </c>
+      <c r="G212" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="H212" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="I212" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="J212" s="117" t="s">
+        <v>449</v>
+      </c>
+      <c r="K212" s="117" t="s">
+        <v>449</v>
+      </c>
+      <c r="L212" s="117" t="s">
+        <v>449</v>
+      </c>
+      <c r="M212" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="N212" s="117" t="s">
+        <v>47</v>
+      </c>
+      <c r="O212" s="120" t="s">
+        <v>48</v>
+      </c>
+      <c r="P212" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q212" s="117" t="s">
+        <v>0</v>
+      </c>
+      <c r="R212" s="117" t="s">
+        <v>1</v>
+      </c>
+      <c r="S212" s="117">
+        <v>1825</v>
+      </c>
+      <c r="T212" s="117" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="213" spans="1:20">
+      <c r="A213" s="123">
+        <v>99096</v>
+      </c>
+      <c r="B213" s="121" t="s">
+        <v>71</v>
+      </c>
+      <c r="C213" s="121" t="s">
+        <v>55</v>
+      </c>
+      <c r="D213" s="121" t="s">
+        <v>23</v>
+      </c>
+      <c r="E213" s="121" t="s">
+        <v>110</v>
+      </c>
+      <c r="F213" s="121" t="s">
+        <v>111</v>
+      </c>
+      <c r="G213" s="119" t="s">
+        <v>433</v>
+      </c>
+      <c r="H213" s="119" t="s">
+        <v>433</v>
+      </c>
+      <c r="I213" s="119" t="s">
+        <v>433</v>
+      </c>
+      <c r="J213" s="117" t="s">
+        <v>449</v>
+      </c>
+      <c r="K213" s="117" t="s">
+        <v>449</v>
+      </c>
+      <c r="L213" s="117" t="s">
+        <v>449</v>
+      </c>
+      <c r="M213" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="N213" s="117" t="s">
+        <v>47</v>
+      </c>
+      <c r="O213" s="120" t="s">
+        <v>48</v>
+      </c>
+      <c r="P213" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q213" s="117" t="s">
+        <v>0</v>
+      </c>
+      <c r="R213" s="117" t="s">
+        <v>1</v>
+      </c>
+      <c r="S213" s="117">
+        <v>1825</v>
+      </c>
+      <c r="T213" s="117" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="218" spans="1:20" s="119" customFormat="1">
       <c r="A218" s="9"/>
@@ -23104,48 +23333,48 @@
       <c r="T220" s="3"/>
     </row>
     <row r="221" spans="1:20" s="119" customFormat="1">
-      <c r="A221" s="123"/>
-      <c r="B221" s="121"/>
-      <c r="C221" s="121"/>
-      <c r="D221" s="121"/>
-      <c r="E221" s="121"/>
-      <c r="F221" s="121"/>
-      <c r="G221" s="121"/>
-      <c r="H221" s="121"/>
-      <c r="I221" s="121"/>
-      <c r="J221" s="121"/>
-      <c r="K221" s="121"/>
-      <c r="L221" s="121"/>
-      <c r="M221" s="121"/>
-      <c r="N221" s="121"/>
-      <c r="O221" s="121"/>
-      <c r="P221" s="121"/>
-      <c r="Q221" s="121"/>
-      <c r="R221" s="121"/>
-      <c r="S221" s="121"/>
-      <c r="T221" s="121"/>
+      <c r="A221" s="9"/>
+      <c r="B221" s="3"/>
+      <c r="C221" s="3"/>
+      <c r="D221" s="3"/>
+      <c r="E221" s="3"/>
+      <c r="F221" s="3"/>
+      <c r="G221" s="3"/>
+      <c r="H221" s="3"/>
+      <c r="I221" s="3"/>
+      <c r="J221" s="3"/>
+      <c r="K221" s="3"/>
+      <c r="L221" s="3"/>
+      <c r="M221" s="3"/>
+      <c r="N221" s="3"/>
+      <c r="O221" s="3"/>
+      <c r="P221" s="3"/>
+      <c r="Q221" s="3"/>
+      <c r="R221" s="3"/>
+      <c r="S221" s="3"/>
+      <c r="T221" s="3"/>
     </row>
     <row r="222" spans="1:20" s="119" customFormat="1">
-      <c r="A222" s="123"/>
-      <c r="B222" s="121"/>
-      <c r="C222" s="121"/>
-      <c r="D222" s="121"/>
-      <c r="E222" s="121"/>
-      <c r="F222" s="121"/>
-      <c r="G222" s="121"/>
-      <c r="H222" s="121"/>
-      <c r="I222" s="121"/>
-      <c r="J222" s="121"/>
-      <c r="K222" s="121"/>
-      <c r="L222" s="121"/>
-      <c r="M222" s="121"/>
-      <c r="N222" s="121"/>
-      <c r="O222" s="121"/>
-      <c r="P222" s="121"/>
-      <c r="Q222" s="121"/>
-      <c r="R222" s="121"/>
-      <c r="S222" s="121"/>
-      <c r="T222" s="121"/>
+      <c r="A222" s="9"/>
+      <c r="B222" s="3"/>
+      <c r="C222" s="3"/>
+      <c r="D222" s="3"/>
+      <c r="E222" s="3"/>
+      <c r="F222" s="3"/>
+      <c r="G222" s="3"/>
+      <c r="H222" s="3"/>
+      <c r="I222" s="3"/>
+      <c r="J222" s="3"/>
+      <c r="K222" s="3"/>
+      <c r="L222" s="3"/>
+      <c r="M222" s="3"/>
+      <c r="N222" s="3"/>
+      <c r="O222" s="3"/>
+      <c r="P222" s="3"/>
+      <c r="Q222" s="3"/>
+      <c r="R222" s="3"/>
+      <c r="S222" s="3"/>
+      <c r="T222" s="3"/>
     </row>
     <row r="223" spans="1:20" s="119" customFormat="1">
       <c r="A223" s="123"/>
@@ -23433,7 +23662,7 @@
       <c r="S235" s="121"/>
       <c r="T235" s="121"/>
     </row>
-    <row r="236" spans="1:20" s="115" customFormat="1">
+    <row r="236" spans="1:20" s="119" customFormat="1">
       <c r="A236" s="123"/>
       <c r="B236" s="121"/>
       <c r="C236" s="121"/>
@@ -23455,7 +23684,7 @@
       <c r="S236" s="121"/>
       <c r="T236" s="121"/>
     </row>
-    <row r="237" spans="1:20" s="115" customFormat="1">
+    <row r="237" spans="1:20" s="119" customFormat="1">
       <c r="A237" s="123"/>
       <c r="B237" s="121"/>
       <c r="C237" s="121"/>
@@ -23544,153 +23773,73 @@
       <c r="T240" s="121"/>
     </row>
     <row r="241" spans="1:20" s="115" customFormat="1">
-      <c r="A241" s="63" t="s">
+      <c r="A241" s="123"/>
+      <c r="B241" s="121"/>
+      <c r="C241" s="121"/>
+      <c r="D241" s="121"/>
+      <c r="E241" s="121"/>
+      <c r="F241" s="121"/>
+      <c r="G241" s="121"/>
+      <c r="H241" s="121"/>
+      <c r="I241" s="121"/>
+      <c r="J241" s="121"/>
+      <c r="K241" s="121"/>
+      <c r="L241" s="121"/>
+      <c r="M241" s="121"/>
+      <c r="N241" s="121"/>
+      <c r="O241" s="121"/>
+      <c r="P241" s="121"/>
+      <c r="Q241" s="121"/>
+      <c r="R241" s="121"/>
+      <c r="S241" s="121"/>
+      <c r="T241" s="121"/>
+    </row>
+    <row r="242" spans="1:20" s="115" customFormat="1">
+      <c r="A242" s="123"/>
+      <c r="B242" s="121"/>
+      <c r="C242" s="121"/>
+      <c r="D242" s="121"/>
+      <c r="E242" s="121"/>
+      <c r="F242" s="121"/>
+      <c r="G242" s="121"/>
+      <c r="H242" s="121"/>
+      <c r="I242" s="121"/>
+      <c r="J242" s="121"/>
+      <c r="K242" s="121"/>
+      <c r="L242" s="121"/>
+      <c r="M242" s="121"/>
+      <c r="N242" s="121"/>
+      <c r="O242" s="121"/>
+      <c r="P242" s="121"/>
+      <c r="Q242" s="121"/>
+      <c r="R242" s="121"/>
+      <c r="S242" s="121"/>
+      <c r="T242" s="121"/>
+    </row>
+    <row r="243" spans="1:20" s="115" customFormat="1">
+      <c r="A243" s="63" t="s">
         <v>450</v>
       </c>
-      <c r="B241" s="116"/>
-      <c r="C241" s="116"/>
-      <c r="D241" s="116"/>
-      <c r="E241" s="116"/>
-      <c r="F241" s="116"/>
-      <c r="J241" s="117"/>
-      <c r="K241" s="117"/>
-      <c r="L241" s="117"/>
-      <c r="M241" s="117"/>
-      <c r="N241" s="117"/>
-      <c r="O241" s="118"/>
-      <c r="P241" s="117"/>
-      <c r="Q241" s="117"/>
-      <c r="R241" s="117"/>
-      <c r="S241" s="117"/>
-      <c r="T241" s="117"/>
-    </row>
-    <row r="242" spans="1:20" s="115" customFormat="1">
-      <c r="A242" s="63" t="s">
+      <c r="B243" s="116"/>
+      <c r="C243" s="116"/>
+      <c r="D243" s="116"/>
+      <c r="E243" s="116"/>
+      <c r="F243" s="116"/>
+      <c r="J243" s="117"/>
+      <c r="K243" s="117"/>
+      <c r="L243" s="117"/>
+      <c r="M243" s="117"/>
+      <c r="N243" s="117"/>
+      <c r="O243" s="118"/>
+      <c r="P243" s="117"/>
+      <c r="Q243" s="117"/>
+      <c r="R243" s="117"/>
+      <c r="S243" s="117"/>
+      <c r="T243" s="117"/>
+    </row>
+    <row r="244" spans="1:20" s="115" customFormat="1">
+      <c r="A244" s="63" t="s">
         <v>451</v>
-      </c>
-      <c r="B242" s="116" t="s">
-        <v>71</v>
-      </c>
-      <c r="C242" s="116" t="s">
-        <v>55</v>
-      </c>
-      <c r="D242" s="116" t="s">
-        <v>443</v>
-      </c>
-      <c r="E242" s="116" t="s">
-        <v>110</v>
-      </c>
-      <c r="F242" s="116" t="s">
-        <v>111</v>
-      </c>
-      <c r="G242" s="117" t="s">
-        <v>35</v>
-      </c>
-      <c r="H242" s="117" t="s">
-        <v>35</v>
-      </c>
-      <c r="I242" s="117" t="s">
-        <v>35</v>
-      </c>
-      <c r="J242" s="117" t="s">
-        <v>445</v>
-      </c>
-      <c r="K242" s="117" t="s">
-        <v>445</v>
-      </c>
-      <c r="L242" s="117" t="s">
-        <v>445</v>
-      </c>
-      <c r="M242" s="117" t="s">
-        <v>22</v>
-      </c>
-      <c r="N242" s="117" t="s">
-        <v>47</v>
-      </c>
-      <c r="O242" s="118" t="s">
-        <v>48</v>
-      </c>
-      <c r="P242" s="117" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q242" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="R242" s="117" t="s">
-        <v>1</v>
-      </c>
-      <c r="S242" s="117">
-        <v>1825</v>
-      </c>
-      <c r="T242" s="117" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="243" spans="1:20" s="77" customFormat="1">
-      <c r="A243" s="63" t="s">
-        <v>452</v>
-      </c>
-      <c r="B243" s="116" t="s">
-        <v>71</v>
-      </c>
-      <c r="C243" s="116" t="s">
-        <v>55</v>
-      </c>
-      <c r="D243" s="116" t="s">
-        <v>444</v>
-      </c>
-      <c r="E243" s="116" t="s">
-        <v>110</v>
-      </c>
-      <c r="F243" s="116" t="s">
-        <v>111</v>
-      </c>
-      <c r="G243" s="117" t="s">
-        <v>34</v>
-      </c>
-      <c r="H243" s="117" t="s">
-        <v>34</v>
-      </c>
-      <c r="I243" s="117" t="s">
-        <v>34</v>
-      </c>
-      <c r="J243" s="117" t="s">
-        <v>445</v>
-      </c>
-      <c r="K243" s="117" t="s">
-        <v>445</v>
-      </c>
-      <c r="L243" s="117" t="s">
-        <v>445</v>
-      </c>
-      <c r="M243" s="117" t="s">
-        <v>22</v>
-      </c>
-      <c r="N243" s="117" t="s">
-        <v>47</v>
-      </c>
-      <c r="O243" s="118" t="s">
-        <v>48</v>
-      </c>
-      <c r="P243" s="117" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q243" s="117" t="s">
-        <v>0</v>
-      </c>
-      <c r="R243" s="117" t="s">
-        <v>1</v>
-      </c>
-      <c r="S243" s="117">
-        <v>1825</v>
-      </c>
-      <c r="T243" s="117" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="244" spans="1:20" s="77" customFormat="1">
-      <c r="A244" s="63" t="s">
-        <v>452</v>
       </c>
       <c r="B244" s="116" t="s">
         <v>71</v>
@@ -23699,7 +23848,7 @@
         <v>55</v>
       </c>
       <c r="D244" s="116" t="s">
-        <v>23</v>
+        <v>443</v>
       </c>
       <c r="E244" s="116" t="s">
         <v>110</v>
@@ -23707,14 +23856,14 @@
       <c r="F244" s="116" t="s">
         <v>111</v>
       </c>
-      <c r="G244" s="115" t="s">
-        <v>433</v>
-      </c>
-      <c r="H244" s="115" t="s">
-        <v>433</v>
-      </c>
-      <c r="I244" s="115" t="s">
-        <v>433</v>
+      <c r="G244" s="117" t="s">
+        <v>35</v>
+      </c>
+      <c r="H244" s="117" t="s">
+        <v>35</v>
+      </c>
+      <c r="I244" s="117" t="s">
+        <v>35</v>
       </c>
       <c r="J244" s="117" t="s">
         <v>445</v>
@@ -23761,7 +23910,7 @@
         <v>55</v>
       </c>
       <c r="D245" s="116" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E245" s="116" t="s">
         <v>110</v>
@@ -23770,22 +23919,22 @@
         <v>111</v>
       </c>
       <c r="G245" s="117" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H245" s="117" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I245" s="117" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J245" s="117" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="K245" s="117" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="L245" s="117" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="M245" s="117" t="s">
         <v>22</v>
@@ -23814,7 +23963,7 @@
     </row>
     <row r="246" spans="1:20" s="77" customFormat="1">
       <c r="A246" s="63" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B246" s="116" t="s">
         <v>71</v>
@@ -23823,7 +23972,7 @@
         <v>55</v>
       </c>
       <c r="D246" s="116" t="s">
-        <v>446</v>
+        <v>23</v>
       </c>
       <c r="E246" s="116" t="s">
         <v>110</v>
@@ -23831,23 +23980,23 @@
       <c r="F246" s="116" t="s">
         <v>111</v>
       </c>
-      <c r="G246" s="117" t="s">
-        <v>34</v>
-      </c>
-      <c r="H246" s="117" t="s">
-        <v>34</v>
-      </c>
-      <c r="I246" s="117" t="s">
-        <v>34</v>
+      <c r="G246" s="115" t="s">
+        <v>433</v>
+      </c>
+      <c r="H246" s="115" t="s">
+        <v>433</v>
+      </c>
+      <c r="I246" s="115" t="s">
+        <v>433</v>
       </c>
       <c r="J246" s="117" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="K246" s="117" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="L246" s="117" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="M246" s="117" t="s">
         <v>22</v>
@@ -23885,7 +24034,7 @@
         <v>55</v>
       </c>
       <c r="D247" s="116" t="s">
-        <v>23</v>
+        <v>446</v>
       </c>
       <c r="E247" s="116" t="s">
         <v>110</v>
@@ -23893,14 +24042,14 @@
       <c r="F247" s="116" t="s">
         <v>111</v>
       </c>
-      <c r="G247" s="115" t="s">
-        <v>433</v>
-      </c>
-      <c r="H247" s="115" t="s">
-        <v>433</v>
-      </c>
-      <c r="I247" s="115" t="s">
-        <v>433</v>
+      <c r="G247" s="117" t="s">
+        <v>35</v>
+      </c>
+      <c r="H247" s="117" t="s">
+        <v>35</v>
+      </c>
+      <c r="I247" s="117" t="s">
+        <v>35</v>
       </c>
       <c r="J247" s="117" t="s">
         <v>449</v>
@@ -23937,141 +24086,179 @@
       </c>
     </row>
     <row r="248" spans="1:20" s="77" customFormat="1">
-      <c r="A248" s="8">
+      <c r="A248" s="63" t="s">
+        <v>453</v>
+      </c>
+      <c r="B248" s="116" t="s">
+        <v>71</v>
+      </c>
+      <c r="C248" s="116" t="s">
+        <v>55</v>
+      </c>
+      <c r="D248" s="116" t="s">
+        <v>446</v>
+      </c>
+      <c r="E248" s="116" t="s">
+        <v>110</v>
+      </c>
+      <c r="F248" s="116" t="s">
+        <v>111</v>
+      </c>
+      <c r="G248" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="H248" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="I248" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="J248" s="117" t="s">
+        <v>449</v>
+      </c>
+      <c r="K248" s="117" t="s">
+        <v>449</v>
+      </c>
+      <c r="L248" s="117" t="s">
+        <v>449</v>
+      </c>
+      <c r="M248" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="N248" s="117" t="s">
+        <v>47</v>
+      </c>
+      <c r="O248" s="118" t="s">
+        <v>48</v>
+      </c>
+      <c r="P248" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q248" s="117" t="s">
+        <v>0</v>
+      </c>
+      <c r="R248" s="117" t="s">
+        <v>1</v>
+      </c>
+      <c r="S248" s="117">
+        <v>1825</v>
+      </c>
+      <c r="T248" s="117" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="249" spans="1:20" s="77" customFormat="1">
+      <c r="A249" s="63" t="s">
+        <v>452</v>
+      </c>
+      <c r="B249" s="116" t="s">
+        <v>71</v>
+      </c>
+      <c r="C249" s="116" t="s">
+        <v>55</v>
+      </c>
+      <c r="D249" s="116" t="s">
+        <v>23</v>
+      </c>
+      <c r="E249" s="116" t="s">
+        <v>110</v>
+      </c>
+      <c r="F249" s="116" t="s">
+        <v>111</v>
+      </c>
+      <c r="G249" s="115" t="s">
+        <v>433</v>
+      </c>
+      <c r="H249" s="115" t="s">
+        <v>433</v>
+      </c>
+      <c r="I249" s="115" t="s">
+        <v>433</v>
+      </c>
+      <c r="J249" s="117" t="s">
+        <v>449</v>
+      </c>
+      <c r="K249" s="117" t="s">
+        <v>449</v>
+      </c>
+      <c r="L249" s="117" t="s">
+        <v>449</v>
+      </c>
+      <c r="M249" s="117" t="s">
+        <v>22</v>
+      </c>
+      <c r="N249" s="117" t="s">
+        <v>47</v>
+      </c>
+      <c r="O249" s="118" t="s">
+        <v>48</v>
+      </c>
+      <c r="P249" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q249" s="117" t="s">
+        <v>0</v>
+      </c>
+      <c r="R249" s="117" t="s">
+        <v>1</v>
+      </c>
+      <c r="S249" s="117">
+        <v>1825</v>
+      </c>
+      <c r="T249" s="117" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="250" spans="1:20" s="77" customFormat="1">
+      <c r="A250" s="8">
         <v>99063</v>
       </c>
-      <c r="B248" s="80" t="s">
+      <c r="B250" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="C248" s="80" t="s">
+      <c r="C250" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="D248" s="81" t="s">
+      <c r="D250" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="E248" s="80" t="s">
+      <c r="E250" s="80" t="s">
         <v>113</v>
       </c>
-      <c r="F248" s="80" t="s">
+      <c r="F250" s="80" t="s">
         <v>418</v>
       </c>
-      <c r="G248" s="81" t="s">
+      <c r="G250" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="H248" s="81" t="s">
+      <c r="H250" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="I248" s="81" t="s">
+      <c r="I250" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="J248" s="80" t="s">
+      <c r="J250" s="80" t="s">
         <v>415</v>
       </c>
-      <c r="K248" s="80" t="s">
+      <c r="K250" s="80" t="s">
         <v>415</v>
       </c>
-      <c r="L248" s="80" t="s">
+      <c r="L250" s="80" t="s">
         <v>415</v>
       </c>
-      <c r="M248" s="81" t="s">
+      <c r="M250" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="N248" s="81" t="s">
+      <c r="N250" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="O248" s="82" t="s">
+      <c r="O250" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="P248" s="81" t="s">
+      <c r="P250" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="Q248" s="81" t="s">
-        <v>0</v>
-      </c>
-      <c r="R248" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="S248" s="81">
-        <v>1825</v>
-      </c>
-      <c r="T248" s="81" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="249" spans="1:20" s="77" customFormat="1">
-      <c r="A249" s="84" t="s">
-        <v>399</v>
-      </c>
-      <c r="B249" s="85"/>
-      <c r="C249" s="85"/>
-      <c r="D249" s="85"/>
-      <c r="E249" s="85"/>
-      <c r="F249" s="85"/>
-      <c r="G249" s="85"/>
-      <c r="H249" s="85"/>
-      <c r="I249" s="85"/>
-      <c r="J249" s="85"/>
-      <c r="K249" s="85"/>
-      <c r="L249" s="85"/>
-      <c r="M249" s="85"/>
-      <c r="N249" s="85"/>
-      <c r="O249" s="86"/>
-      <c r="P249" s="85"/>
-      <c r="Q249" s="85"/>
-      <c r="R249" s="81"/>
-      <c r="S249" s="81"/>
-      <c r="T249" s="81"/>
-    </row>
-    <row r="250" spans="1:20" s="77" customFormat="1">
-      <c r="A250" s="87">
-        <v>99061</v>
-      </c>
-      <c r="B250" s="85" t="s">
-        <v>71</v>
-      </c>
-      <c r="C250" s="85" t="s">
-        <v>55</v>
-      </c>
-      <c r="D250" s="85" t="s">
-        <v>365</v>
-      </c>
-      <c r="E250" s="85" t="s">
-        <v>376</v>
-      </c>
-      <c r="F250" s="85" t="s">
-        <v>375</v>
-      </c>
-      <c r="G250" s="85" t="s">
-        <v>35</v>
-      </c>
-      <c r="H250" s="85" t="s">
-        <v>35</v>
-      </c>
-      <c r="I250" s="85" t="s">
-        <v>35</v>
-      </c>
-      <c r="J250" s="85" t="s">
-        <v>360</v>
-      </c>
-      <c r="K250" s="85" t="s">
-        <v>360</v>
-      </c>
-      <c r="L250" s="85" t="s">
-        <v>360</v>
-      </c>
-      <c r="M250" s="85" t="s">
-        <v>22</v>
-      </c>
-      <c r="N250" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="O250" s="86" t="s">
-        <v>48</v>
-      </c>
-      <c r="P250" s="85" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q250" s="85" t="s">
+      <c r="Q250" s="81" t="s">
         <v>0</v>
       </c>
       <c r="R250" s="81" t="s">
@@ -24085,70 +24272,32 @@
       </c>
     </row>
     <row r="251" spans="1:20" s="77" customFormat="1">
-      <c r="A251" s="87">
-        <v>99062</v>
-      </c>
-      <c r="B251" s="85" t="s">
-        <v>71</v>
-      </c>
-      <c r="C251" s="85" t="s">
-        <v>55</v>
-      </c>
-      <c r="D251" s="85" t="s">
-        <v>365</v>
-      </c>
-      <c r="E251" s="85" t="s">
-        <v>376</v>
-      </c>
-      <c r="F251" s="85" t="s">
-        <v>379</v>
-      </c>
-      <c r="G251" s="85" t="s">
-        <v>35</v>
-      </c>
-      <c r="H251" s="85" t="s">
-        <v>35</v>
-      </c>
-      <c r="I251" s="85" t="s">
-        <v>35</v>
-      </c>
-      <c r="J251" s="85" t="s">
-        <v>360</v>
-      </c>
-      <c r="K251" s="85" t="s">
-        <v>360</v>
-      </c>
-      <c r="L251" s="85" t="s">
-        <v>360</v>
-      </c>
-      <c r="M251" s="85" t="s">
-        <v>22</v>
-      </c>
-      <c r="N251" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="O251" s="86" t="s">
-        <v>48</v>
-      </c>
-      <c r="P251" s="85" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q251" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="R251" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="S251" s="81">
-        <v>1825</v>
-      </c>
-      <c r="T251" s="81" t="s">
-        <v>25</v>
-      </c>
+      <c r="A251" s="84" t="s">
+        <v>399</v>
+      </c>
+      <c r="B251" s="85"/>
+      <c r="C251" s="85"/>
+      <c r="D251" s="85"/>
+      <c r="E251" s="85"/>
+      <c r="F251" s="85"/>
+      <c r="G251" s="85"/>
+      <c r="H251" s="85"/>
+      <c r="I251" s="85"/>
+      <c r="J251" s="85"/>
+      <c r="K251" s="85"/>
+      <c r="L251" s="85"/>
+      <c r="M251" s="85"/>
+      <c r="N251" s="85"/>
+      <c r="O251" s="86"/>
+      <c r="P251" s="85"/>
+      <c r="Q251" s="85"/>
+      <c r="R251" s="81"/>
+      <c r="S251" s="81"/>
+      <c r="T251" s="81"/>
     </row>
     <row r="252" spans="1:20" s="77" customFormat="1">
       <c r="A252" s="87">
-        <v>99063</v>
+        <v>99061</v>
       </c>
       <c r="B252" s="85" t="s">
         <v>71</v>
@@ -24163,7 +24312,7 @@
         <v>376</v>
       </c>
       <c r="F252" s="85" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="G252" s="85" t="s">
         <v>35</v>
@@ -24210,7 +24359,7 @@
     </row>
     <row r="253" spans="1:20" s="77" customFormat="1">
       <c r="A253" s="87">
-        <v>99064</v>
+        <v>99062</v>
       </c>
       <c r="B253" s="85" t="s">
         <v>71</v>
@@ -24225,7 +24374,7 @@
         <v>376</v>
       </c>
       <c r="F253" s="85" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="G253" s="85" t="s">
         <v>35</v>
@@ -24272,7 +24421,7 @@
     </row>
     <row r="254" spans="1:20" s="77" customFormat="1">
       <c r="A254" s="87">
-        <v>99061</v>
+        <v>99063</v>
       </c>
       <c r="B254" s="85" t="s">
         <v>71</v>
@@ -24287,7 +24436,7 @@
         <v>376</v>
       </c>
       <c r="F254" s="85" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="G254" s="85" t="s">
         <v>35</v>
@@ -24334,7 +24483,7 @@
     </row>
     <row r="255" spans="1:20" s="77" customFormat="1">
       <c r="A255" s="87">
-        <v>99062</v>
+        <v>99064</v>
       </c>
       <c r="B255" s="85" t="s">
         <v>71</v>
@@ -24349,7 +24498,7 @@
         <v>376</v>
       </c>
       <c r="F255" s="85" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="G255" s="85" t="s">
         <v>35</v>
@@ -24396,7 +24545,7 @@
     </row>
     <row r="256" spans="1:20" s="77" customFormat="1">
       <c r="A256" s="87">
-        <v>99063</v>
+        <v>99061</v>
       </c>
       <c r="B256" s="85" t="s">
         <v>71</v>
@@ -24411,7 +24560,7 @@
         <v>376</v>
       </c>
       <c r="F256" s="85" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="G256" s="85" t="s">
         <v>35</v>
@@ -24456,9 +24605,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="257" spans="1:22" s="77" customFormat="1">
+    <row r="257" spans="1:20" s="77" customFormat="1">
       <c r="A257" s="87">
-        <v>99064</v>
+        <v>99062</v>
       </c>
       <c r="B257" s="85" t="s">
         <v>71</v>
@@ -24473,7 +24622,7 @@
         <v>376</v>
       </c>
       <c r="F257" s="85" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="G257" s="85" t="s">
         <v>35</v>
@@ -24518,33 +24667,71 @@
         <v>25</v>
       </c>
     </row>
-    <row r="258" spans="1:22" s="77" customFormat="1">
-      <c r="A258" s="84" t="s">
-        <v>402</v>
-      </c>
-      <c r="B258" s="85"/>
-      <c r="C258" s="85"/>
-      <c r="D258" s="85"/>
-      <c r="E258" s="85"/>
-      <c r="F258" s="85"/>
-      <c r="G258" s="85"/>
-      <c r="H258" s="85"/>
-      <c r="I258" s="85"/>
-      <c r="J258" s="85"/>
-      <c r="K258" s="85"/>
-      <c r="L258" s="85"/>
-      <c r="M258" s="85"/>
-      <c r="N258" s="85"/>
-      <c r="O258" s="86"/>
-      <c r="P258" s="85"/>
-      <c r="Q258" s="85"/>
-      <c r="R258" s="81"/>
-      <c r="S258" s="81"/>
-      <c r="T258" s="81"/>
-    </row>
-    <row r="259" spans="1:22">
-      <c r="A259" s="84">
-        <v>99060</v>
+    <row r="258" spans="1:20" s="77" customFormat="1">
+      <c r="A258" s="87">
+        <v>99063</v>
+      </c>
+      <c r="B258" s="85" t="s">
+        <v>71</v>
+      </c>
+      <c r="C258" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="D258" s="85" t="s">
+        <v>365</v>
+      </c>
+      <c r="E258" s="85" t="s">
+        <v>376</v>
+      </c>
+      <c r="F258" s="85" t="s">
+        <v>385</v>
+      </c>
+      <c r="G258" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="H258" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="I258" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="J258" s="85" t="s">
+        <v>360</v>
+      </c>
+      <c r="K258" s="85" t="s">
+        <v>360</v>
+      </c>
+      <c r="L258" s="85" t="s">
+        <v>360</v>
+      </c>
+      <c r="M258" s="85" t="s">
+        <v>22</v>
+      </c>
+      <c r="N258" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="O258" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="P258" s="85" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q258" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="R258" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="S258" s="81">
+        <v>1825</v>
+      </c>
+      <c r="T258" s="81" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="259" spans="1:20" s="77" customFormat="1">
+      <c r="A259" s="87">
+        <v>99064</v>
       </c>
       <c r="B259" s="85" t="s">
         <v>71</v>
@@ -24556,10 +24743,10 @@
         <v>365</v>
       </c>
       <c r="E259" s="85" t="s">
-        <v>110</v>
+        <v>376</v>
       </c>
       <c r="F259" s="85" t="s">
-        <v>111</v>
+        <v>386</v>
       </c>
       <c r="G259" s="85" t="s">
         <v>35</v>
@@ -24579,8 +24766,8 @@
       <c r="L259" s="85" t="s">
         <v>360</v>
       </c>
-      <c r="M259" s="88" t="s">
-        <v>400</v>
+      <c r="M259" s="85" t="s">
+        <v>22</v>
       </c>
       <c r="N259" s="85" t="s">
         <v>47</v>
@@ -24604,9 +24791,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="260" spans="1:22" s="77" customFormat="1">
+    <row r="260" spans="1:20" s="77" customFormat="1">
       <c r="A260" s="84" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B260" s="85"/>
       <c r="C260" s="85"/>
@@ -24628,9 +24815,9 @@
       <c r="S260" s="81"/>
       <c r="T260" s="81"/>
     </row>
-    <row r="261" spans="1:22" s="77" customFormat="1">
+    <row r="261" spans="1:20">
       <c r="A261" s="84">
-        <v>99061</v>
+        <v>99060</v>
       </c>
       <c r="B261" s="85" t="s">
         <v>71</v>
@@ -24639,13 +24826,13 @@
         <v>55</v>
       </c>
       <c r="D261" s="85" t="s">
-        <v>23</v>
+        <v>365</v>
       </c>
       <c r="E261" s="85" t="s">
-        <v>377</v>
+        <v>110</v>
       </c>
       <c r="F261" s="85" t="s">
-        <v>378</v>
+        <v>111</v>
       </c>
       <c r="G261" s="85" t="s">
         <v>35</v>
@@ -24666,7 +24853,7 @@
         <v>360</v>
       </c>
       <c r="M261" s="88" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="N261" s="85" t="s">
         <v>47</v>
@@ -24690,9 +24877,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="262" spans="1:22" s="77" customFormat="1">
+    <row r="262" spans="1:20" s="77" customFormat="1">
       <c r="A262" s="84" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="B262" s="85"/>
       <c r="C262" s="85"/>
@@ -24714,9 +24901,9 @@
       <c r="S262" s="81"/>
       <c r="T262" s="81"/>
     </row>
-    <row r="263" spans="1:22" s="77" customFormat="1">
+    <row r="263" spans="1:20" s="77" customFormat="1">
       <c r="A263" s="84">
-        <v>99062</v>
+        <v>99061</v>
       </c>
       <c r="B263" s="85" t="s">
         <v>71</v>
@@ -24725,13 +24912,13 @@
         <v>55</v>
       </c>
       <c r="D263" s="85" t="s">
-        <v>406</v>
+        <v>23</v>
       </c>
       <c r="E263" s="85" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="F263" s="85" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="G263" s="85" t="s">
         <v>35</v>
@@ -24776,9 +24963,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="264" spans="1:22" s="77" customFormat="1">
+    <row r="264" spans="1:20" s="77" customFormat="1">
       <c r="A264" s="84" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B264" s="85"/>
       <c r="C264" s="85"/>
@@ -24793,16 +24980,16 @@
       <c r="L264" s="85"/>
       <c r="M264" s="85"/>
       <c r="N264" s="85"/>
-      <c r="O264" s="85"/>
+      <c r="O264" s="86"/>
       <c r="P264" s="85"/>
       <c r="Q264" s="85"/>
-      <c r="R264" s="3"/>
-      <c r="S264" s="3"/>
-      <c r="T264" s="3"/>
-    </row>
-    <row r="265" spans="1:22" s="77" customFormat="1" ht="13.5" customHeight="1">
+      <c r="R264" s="81"/>
+      <c r="S264" s="81"/>
+      <c r="T264" s="81"/>
+    </row>
+    <row r="265" spans="1:20" s="77" customFormat="1">
       <c r="A265" s="84">
-        <v>99070</v>
+        <v>99062</v>
       </c>
       <c r="B265" s="85" t="s">
         <v>71</v>
@@ -24811,13 +24998,13 @@
         <v>55</v>
       </c>
       <c r="D265" s="85" t="s">
-        <v>388</v>
+        <v>406</v>
       </c>
       <c r="E265" s="85" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F265" s="85" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="G265" s="85" t="s">
         <v>35</v>
@@ -24862,71 +25049,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="266" spans="1:22" s="77" customFormat="1">
-      <c r="A266" s="84">
-        <v>99071</v>
-      </c>
-      <c r="B266" s="85" t="s">
-        <v>71</v>
-      </c>
-      <c r="C266" s="85" t="s">
-        <v>55</v>
-      </c>
-      <c r="D266" s="85" t="s">
-        <v>388</v>
-      </c>
-      <c r="E266" s="85" t="s">
-        <v>394</v>
-      </c>
-      <c r="F266" s="85" t="s">
-        <v>381</v>
-      </c>
-      <c r="G266" s="85" t="s">
-        <v>35</v>
-      </c>
-      <c r="H266" s="85" t="s">
-        <v>35</v>
-      </c>
-      <c r="I266" s="85" t="s">
-        <v>35</v>
-      </c>
-      <c r="J266" s="85" t="s">
-        <v>360</v>
-      </c>
-      <c r="K266" s="85" t="s">
-        <v>360</v>
-      </c>
-      <c r="L266" s="85" t="s">
-        <v>360</v>
-      </c>
-      <c r="M266" s="88" t="s">
-        <v>387</v>
-      </c>
-      <c r="N266" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="O266" s="86" t="s">
-        <v>48</v>
-      </c>
-      <c r="P266" s="85" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q266" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="R266" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="S266" s="81">
-        <v>1825</v>
-      </c>
-      <c r="T266" s="81" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="267" spans="1:22" s="77" customFormat="1">
+    <row r="266" spans="1:20" s="77" customFormat="1">
+      <c r="A266" s="84" t="s">
+        <v>396</v>
+      </c>
+      <c r="B266" s="85"/>
+      <c r="C266" s="85"/>
+      <c r="D266" s="85"/>
+      <c r="E266" s="85"/>
+      <c r="F266" s="85"/>
+      <c r="G266" s="85"/>
+      <c r="H266" s="85"/>
+      <c r="I266" s="85"/>
+      <c r="J266" s="85"/>
+      <c r="K266" s="85"/>
+      <c r="L266" s="85"/>
+      <c r="M266" s="85"/>
+      <c r="N266" s="85"/>
+      <c r="O266" s="85"/>
+      <c r="P266" s="85"/>
+      <c r="Q266" s="85"/>
+      <c r="R266" s="3"/>
+      <c r="S266" s="3"/>
+      <c r="T266" s="3"/>
+    </row>
+    <row r="267" spans="1:20" s="77" customFormat="1" ht="13.5" customHeight="1">
       <c r="A267" s="84">
-        <v>99072</v>
+        <v>99070</v>
       </c>
       <c r="B267" s="85" t="s">
         <v>71</v>
@@ -24938,10 +25087,10 @@
         <v>388</v>
       </c>
       <c r="E267" s="85" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="F267" s="85" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="G267" s="85" t="s">
         <v>35</v>
@@ -24986,9 +25135,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="268" spans="1:22" s="77" customFormat="1">
+    <row r="268" spans="1:20" s="77" customFormat="1">
       <c r="A268" s="84">
-        <v>99073</v>
+        <v>99071</v>
       </c>
       <c r="B268" s="85" t="s">
         <v>71</v>
@@ -25000,10 +25149,10 @@
         <v>388</v>
       </c>
       <c r="E268" s="85" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F268" s="85" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G268" s="85" t="s">
         <v>35</v>
@@ -25048,31 +25197,71 @@
         <v>25</v>
       </c>
     </row>
-    <row r="269" spans="1:22" s="77" customFormat="1">
-      <c r="A269" s="84"/>
-      <c r="B269" s="85"/>
-      <c r="C269" s="85"/>
-      <c r="D269" s="85"/>
-      <c r="E269" s="85"/>
-      <c r="F269" s="85"/>
-      <c r="G269" s="85"/>
-      <c r="H269" s="85"/>
-      <c r="I269" s="85"/>
-      <c r="J269" s="85"/>
-      <c r="K269" s="85"/>
-      <c r="L269" s="85"/>
-      <c r="M269" s="85"/>
-      <c r="N269" s="85"/>
-      <c r="O269" s="85"/>
-      <c r="P269" s="85"/>
-      <c r="Q269" s="85"/>
-      <c r="R269" s="80"/>
-      <c r="S269" s="80"/>
-      <c r="T269" s="80"/>
-    </row>
-    <row r="270" spans="1:22">
+    <row r="269" spans="1:20" s="77" customFormat="1">
+      <c r="A269" s="84">
+        <v>99072</v>
+      </c>
+      <c r="B269" s="85" t="s">
+        <v>71</v>
+      </c>
+      <c r="C269" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="D269" s="85" t="s">
+        <v>388</v>
+      </c>
+      <c r="E269" s="85" t="s">
+        <v>382</v>
+      </c>
+      <c r="F269" s="85" t="s">
+        <v>383</v>
+      </c>
+      <c r="G269" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="H269" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="I269" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="J269" s="85" t="s">
+        <v>360</v>
+      </c>
+      <c r="K269" s="85" t="s">
+        <v>360</v>
+      </c>
+      <c r="L269" s="85" t="s">
+        <v>360</v>
+      </c>
+      <c r="M269" s="88" t="s">
+        <v>387</v>
+      </c>
+      <c r="N269" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="O269" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="P269" s="85" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q269" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="R269" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="S269" s="81">
+        <v>1825</v>
+      </c>
+      <c r="T269" s="81" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="270" spans="1:20" s="77" customFormat="1">
       <c r="A270" s="84">
-        <v>99066</v>
+        <v>99073</v>
       </c>
       <c r="B270" s="85" t="s">
         <v>71</v>
@@ -25084,10 +25273,10 @@
         <v>388</v>
       </c>
       <c r="E270" s="85" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="F270" s="85" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="G270" s="85" t="s">
         <v>35</v>
@@ -25107,8 +25296,8 @@
       <c r="L270" s="85" t="s">
         <v>360</v>
       </c>
-      <c r="M270" s="85" t="s">
-        <v>22</v>
+      <c r="M270" s="88" t="s">
+        <v>387</v>
       </c>
       <c r="N270" s="85" t="s">
         <v>47</v>
@@ -25132,73 +25321,31 @@
         <v>25</v>
       </c>
     </row>
-    <row r="271" spans="1:22">
-      <c r="A271" s="84">
-        <v>99067</v>
-      </c>
-      <c r="B271" s="85" t="s">
-        <v>71</v>
-      </c>
-      <c r="C271" s="85" t="s">
-        <v>55</v>
-      </c>
-      <c r="D271" s="85" t="s">
-        <v>388</v>
-      </c>
-      <c r="E271" s="85" t="s">
-        <v>392</v>
-      </c>
-      <c r="F271" s="85" t="s">
-        <v>381</v>
-      </c>
-      <c r="G271" s="85" t="s">
-        <v>35</v>
-      </c>
-      <c r="H271" s="85" t="s">
-        <v>35</v>
-      </c>
-      <c r="I271" s="85" t="s">
-        <v>35</v>
-      </c>
-      <c r="J271" s="85" t="s">
-        <v>360</v>
-      </c>
-      <c r="K271" s="85" t="s">
-        <v>360</v>
-      </c>
-      <c r="L271" s="85" t="s">
-        <v>360</v>
-      </c>
-      <c r="M271" s="85" t="s">
-        <v>22</v>
-      </c>
-      <c r="N271" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="O271" s="86" t="s">
-        <v>48</v>
-      </c>
-      <c r="P271" s="85" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q271" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="R271" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="S271" s="81">
-        <v>1825</v>
-      </c>
-      <c r="T271" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="U271" s="66"/>
-      <c r="V271" s="66"/>
-    </row>
-    <row r="272" spans="1:22">
+    <row r="271" spans="1:20" s="77" customFormat="1">
+      <c r="A271" s="84"/>
+      <c r="B271" s="85"/>
+      <c r="C271" s="85"/>
+      <c r="D271" s="85"/>
+      <c r="E271" s="85"/>
+      <c r="F271" s="85"/>
+      <c r="G271" s="85"/>
+      <c r="H271" s="85"/>
+      <c r="I271" s="85"/>
+      <c r="J271" s="85"/>
+      <c r="K271" s="85"/>
+      <c r="L271" s="85"/>
+      <c r="M271" s="85"/>
+      <c r="N271" s="85"/>
+      <c r="O271" s="85"/>
+      <c r="P271" s="85"/>
+      <c r="Q271" s="85"/>
+      <c r="R271" s="80"/>
+      <c r="S271" s="80"/>
+      <c r="T271" s="80"/>
+    </row>
+    <row r="272" spans="1:20">
       <c r="A272" s="84">
-        <v>99068</v>
+        <v>99066</v>
       </c>
       <c r="B272" s="85" t="s">
         <v>71</v>
@@ -25210,10 +25357,10 @@
         <v>388</v>
       </c>
       <c r="E272" s="85" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="F272" s="85" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="G272" s="85" t="s">
         <v>35</v>
@@ -25257,12 +25404,10 @@
       <c r="T272" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="U272" s="66"/>
-      <c r="V272" s="66"/>
     </row>
     <row r="273" spans="1:22">
       <c r="A273" s="84">
-        <v>99069</v>
+        <v>99067</v>
       </c>
       <c r="B273" s="85" t="s">
         <v>71</v>
@@ -25274,10 +25419,10 @@
         <v>388</v>
       </c>
       <c r="E273" s="85" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F273" s="85" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G273" s="85" t="s">
         <v>35</v>
@@ -25325,54 +25470,135 @@
       <c r="V273" s="66"/>
     </row>
     <row r="274" spans="1:22">
-      <c r="A274" s="84"/>
-      <c r="B274" s="85"/>
-      <c r="C274" s="85"/>
-      <c r="D274" s="85"/>
-      <c r="E274" s="85"/>
-      <c r="F274" s="85"/>
-      <c r="G274" s="85"/>
-      <c r="H274" s="85"/>
-      <c r="I274" s="85"/>
-      <c r="J274" s="85"/>
-      <c r="K274" s="85"/>
-      <c r="L274" s="85"/>
-      <c r="M274" s="85"/>
-      <c r="N274" s="85"/>
-      <c r="O274" s="85"/>
-      <c r="P274" s="85"/>
-      <c r="Q274" s="85"/>
-      <c r="R274" s="80"/>
-      <c r="S274" s="80"/>
-      <c r="T274" s="80"/>
+      <c r="A274" s="84">
+        <v>99068</v>
+      </c>
+      <c r="B274" s="85" t="s">
+        <v>71</v>
+      </c>
+      <c r="C274" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="D274" s="85" t="s">
+        <v>388</v>
+      </c>
+      <c r="E274" s="85" t="s">
+        <v>382</v>
+      </c>
+      <c r="F274" s="85" t="s">
+        <v>383</v>
+      </c>
+      <c r="G274" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="H274" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="I274" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="J274" s="85" t="s">
+        <v>360</v>
+      </c>
+      <c r="K274" s="85" t="s">
+        <v>360</v>
+      </c>
+      <c r="L274" s="85" t="s">
+        <v>360</v>
+      </c>
+      <c r="M274" s="85" t="s">
+        <v>22</v>
+      </c>
+      <c r="N274" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="O274" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="P274" s="85" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q274" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="R274" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="S274" s="81">
+        <v>1825</v>
+      </c>
+      <c r="T274" s="81" t="s">
+        <v>25</v>
+      </c>
       <c r="U274" s="66"/>
       <c r="V274" s="66"/>
     </row>
     <row r="275" spans="1:22">
-      <c r="A275" s="84"/>
-      <c r="B275" s="85"/>
-      <c r="C275" s="85"/>
-      <c r="D275" s="85"/>
-      <c r="E275" s="85"/>
-      <c r="F275" s="85"/>
-      <c r="G275" s="85"/>
-      <c r="H275" s="85"/>
-      <c r="I275" s="85"/>
-      <c r="J275" s="85"/>
-      <c r="K275" s="85"/>
-      <c r="L275" s="85"/>
-      <c r="M275" s="85"/>
-      <c r="N275" s="85"/>
-      <c r="O275" s="85"/>
-      <c r="P275" s="85"/>
-      <c r="Q275" s="85"/>
+      <c r="A275" s="84">
+        <v>99069</v>
+      </c>
+      <c r="B275" s="85" t="s">
+        <v>71</v>
+      </c>
+      <c r="C275" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="D275" s="85" t="s">
+        <v>388</v>
+      </c>
+      <c r="E275" s="85" t="s">
+        <v>393</v>
+      </c>
+      <c r="F275" s="85" t="s">
+        <v>384</v>
+      </c>
+      <c r="G275" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="H275" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="I275" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="J275" s="85" t="s">
+        <v>360</v>
+      </c>
+      <c r="K275" s="85" t="s">
+        <v>360</v>
+      </c>
+      <c r="L275" s="85" t="s">
+        <v>360</v>
+      </c>
+      <c r="M275" s="85" t="s">
+        <v>22</v>
+      </c>
+      <c r="N275" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="O275" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="P275" s="85" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q275" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="R275" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="S275" s="81">
+        <v>1825</v>
+      </c>
+      <c r="T275" s="81" t="s">
+        <v>25</v>
+      </c>
       <c r="U275" s="66"/>
       <c r="V275" s="66"/>
     </row>
     <row r="276" spans="1:22">
-      <c r="A276" s="84" t="s">
-        <v>248</v>
-      </c>
+      <c r="A276" s="84"/>
       <c r="B276" s="85"/>
       <c r="C276" s="85"/>
       <c r="D276" s="85"/>
@@ -25389,13 +25615,14 @@
       <c r="O276" s="85"/>
       <c r="P276" s="85"/>
       <c r="Q276" s="85"/>
+      <c r="R276" s="80"/>
+      <c r="S276" s="80"/>
+      <c r="T276" s="80"/>
       <c r="U276" s="66"/>
       <c r="V276" s="66"/>
     </row>
-    <row r="277" spans="1:22" s="64" customFormat="1">
-      <c r="A277" s="84" t="s">
-        <v>257</v>
-      </c>
+    <row r="277" spans="1:22">
+      <c r="A277" s="84"/>
       <c r="B277" s="85"/>
       <c r="C277" s="85"/>
       <c r="D277" s="85"/>
@@ -25412,143 +25639,61 @@
       <c r="O277" s="85"/>
       <c r="P277" s="85"/>
       <c r="Q277" s="85"/>
-      <c r="R277" s="3"/>
-      <c r="S277" s="3"/>
-      <c r="T277" s="3"/>
       <c r="U277" s="66"/>
       <c r="V277" s="66"/>
     </row>
-    <row r="278" spans="1:22" s="64" customFormat="1">
-      <c r="A278" s="84">
-        <v>80001</v>
-      </c>
-      <c r="B278" s="85" t="s">
-        <v>260</v>
-      </c>
-      <c r="C278" s="85" t="s">
-        <v>55</v>
-      </c>
-      <c r="D278" s="85" t="s">
-        <v>263</v>
-      </c>
-      <c r="E278" s="85" t="s">
-        <v>249</v>
-      </c>
-      <c r="F278" s="85" t="s">
-        <v>250</v>
-      </c>
-      <c r="G278" s="85" t="s">
-        <v>261</v>
-      </c>
-      <c r="H278" s="85" t="s">
-        <v>249</v>
-      </c>
-      <c r="I278" s="85" t="s">
-        <v>249</v>
-      </c>
-      <c r="J278" s="85" t="s">
-        <v>259</v>
-      </c>
-      <c r="K278" s="85" t="s">
-        <v>31</v>
-      </c>
-      <c r="L278" s="85" t="s">
-        <v>31</v>
-      </c>
-      <c r="M278" s="85" t="s">
-        <v>251</v>
-      </c>
-      <c r="N278" s="85" t="s">
-        <v>263</v>
-      </c>
-      <c r="O278" s="86" t="s">
-        <v>48</v>
-      </c>
-      <c r="P278" s="85" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q278" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="R278" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="S278" s="68">
-        <v>1825</v>
-      </c>
-      <c r="T278" s="65" t="s">
-        <v>25</v>
-      </c>
+    <row r="278" spans="1:22">
+      <c r="A278" s="84" t="s">
+        <v>248</v>
+      </c>
+      <c r="B278" s="85"/>
+      <c r="C278" s="85"/>
+      <c r="D278" s="85"/>
+      <c r="E278" s="85"/>
+      <c r="F278" s="85"/>
+      <c r="G278" s="85"/>
+      <c r="H278" s="85"/>
+      <c r="I278" s="85"/>
+      <c r="J278" s="85"/>
+      <c r="K278" s="85"/>
+      <c r="L278" s="85"/>
+      <c r="M278" s="85"/>
+      <c r="N278" s="85"/>
+      <c r="O278" s="85"/>
+      <c r="P278" s="85"/>
+      <c r="Q278" s="85"/>
       <c r="U278" s="66"/>
       <c r="V278" s="66"/>
     </row>
     <row r="279" spans="1:22" s="64" customFormat="1">
-      <c r="A279" s="84">
-        <v>80012</v>
-      </c>
-      <c r="B279" s="85" t="s">
-        <v>260</v>
-      </c>
-      <c r="C279" s="85" t="s">
-        <v>55</v>
-      </c>
-      <c r="D279" s="85" t="s">
-        <v>264</v>
-      </c>
-      <c r="E279" s="85" t="s">
-        <v>249</v>
-      </c>
-      <c r="F279" s="85" t="s">
-        <v>250</v>
-      </c>
-      <c r="G279" s="85" t="s">
-        <v>262</v>
-      </c>
-      <c r="H279" s="85" t="s">
-        <v>249</v>
-      </c>
-      <c r="I279" s="85" t="s">
-        <v>249</v>
-      </c>
-      <c r="J279" s="85" t="s">
-        <v>259</v>
-      </c>
-      <c r="K279" s="85" t="s">
-        <v>31</v>
-      </c>
-      <c r="L279" s="85" t="s">
-        <v>31</v>
-      </c>
-      <c r="M279" s="85" t="s">
-        <v>251</v>
-      </c>
-      <c r="N279" s="85" t="s">
-        <v>264</v>
-      </c>
-      <c r="O279" s="86" t="s">
-        <v>48</v>
-      </c>
-      <c r="P279" s="85" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q279" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="R279" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="S279" s="68">
-        <v>1825</v>
-      </c>
-      <c r="T279" s="65" t="s">
-        <v>25</v>
-      </c>
+      <c r="A279" s="84" t="s">
+        <v>257</v>
+      </c>
+      <c r="B279" s="85"/>
+      <c r="C279" s="85"/>
+      <c r="D279" s="85"/>
+      <c r="E279" s="85"/>
+      <c r="F279" s="85"/>
+      <c r="G279" s="85"/>
+      <c r="H279" s="85"/>
+      <c r="I279" s="85"/>
+      <c r="J279" s="85"/>
+      <c r="K279" s="85"/>
+      <c r="L279" s="85"/>
+      <c r="M279" s="85"/>
+      <c r="N279" s="85"/>
+      <c r="O279" s="85"/>
+      <c r="P279" s="85"/>
+      <c r="Q279" s="85"/>
+      <c r="R279" s="3"/>
+      <c r="S279" s="3"/>
+      <c r="T279" s="3"/>
       <c r="U279" s="66"/>
       <c r="V279" s="66"/>
     </row>
-    <row r="280" spans="1:22">
+    <row r="280" spans="1:22" s="64" customFormat="1">
       <c r="A280" s="84">
-        <v>80123</v>
+        <v>80001</v>
       </c>
       <c r="B280" s="85" t="s">
         <v>260</v>
@@ -25557,7 +25702,7 @@
         <v>55</v>
       </c>
       <c r="D280" s="85" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="E280" s="85" t="s">
         <v>249</v>
@@ -25566,7 +25711,7 @@
         <v>250</v>
       </c>
       <c r="G280" s="85" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H280" s="85" t="s">
         <v>249</v>
@@ -25587,7 +25732,7 @@
         <v>251</v>
       </c>
       <c r="N280" s="85" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="O280" s="86" t="s">
         <v>48</v>
@@ -25607,31 +25752,76 @@
       <c r="T280" s="65" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="281" spans="1:22">
-      <c r="A281" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="B281" s="85"/>
-      <c r="C281" s="85"/>
-      <c r="D281" s="85"/>
-      <c r="E281" s="85"/>
-      <c r="F281" s="85"/>
-      <c r="G281" s="85"/>
-      <c r="H281" s="85"/>
-      <c r="I281" s="85"/>
-      <c r="J281" s="85"/>
-      <c r="K281" s="85"/>
-      <c r="L281" s="85"/>
-      <c r="M281" s="85"/>
-      <c r="N281" s="85"/>
-      <c r="O281" s="85"/>
-      <c r="P281" s="85"/>
-      <c r="Q281" s="85"/>
+      <c r="U280" s="66"/>
+      <c r="V280" s="66"/>
+    </row>
+    <row r="281" spans="1:22" s="64" customFormat="1">
+      <c r="A281" s="84">
+        <v>80012</v>
+      </c>
+      <c r="B281" s="85" t="s">
+        <v>260</v>
+      </c>
+      <c r="C281" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="D281" s="85" t="s">
+        <v>264</v>
+      </c>
+      <c r="E281" s="85" t="s">
+        <v>249</v>
+      </c>
+      <c r="F281" s="85" t="s">
+        <v>250</v>
+      </c>
+      <c r="G281" s="85" t="s">
+        <v>262</v>
+      </c>
+      <c r="H281" s="85" t="s">
+        <v>249</v>
+      </c>
+      <c r="I281" s="85" t="s">
+        <v>249</v>
+      </c>
+      <c r="J281" s="85" t="s">
+        <v>259</v>
+      </c>
+      <c r="K281" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="L281" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="M281" s="85" t="s">
+        <v>251</v>
+      </c>
+      <c r="N281" s="85" t="s">
+        <v>264</v>
+      </c>
+      <c r="O281" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="P281" s="85" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q281" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="R281" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="S281" s="68">
+        <v>1825</v>
+      </c>
+      <c r="T281" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="U281" s="66"/>
+      <c r="V281" s="66"/>
     </row>
     <row r="282" spans="1:22">
       <c r="A282" s="84">
-        <v>90001</v>
+        <v>80123</v>
       </c>
       <c r="B282" s="85" t="s">
         <v>260</v>
@@ -25640,7 +25830,7 @@
         <v>55</v>
       </c>
       <c r="D282" s="85" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E282" s="85" t="s">
         <v>249</v>
@@ -25667,10 +25857,10 @@
         <v>31</v>
       </c>
       <c r="M282" s="85" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="N282" s="85" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="O282" s="86" t="s">
         <v>48</v>
@@ -25692,70 +25882,29 @@
       </c>
     </row>
     <row r="283" spans="1:22">
-      <c r="A283" s="84">
-        <v>90012</v>
-      </c>
-      <c r="B283" s="85" t="s">
-        <v>260</v>
-      </c>
-      <c r="C283" s="85" t="s">
-        <v>55</v>
-      </c>
-      <c r="D283" s="85" t="s">
-        <v>254</v>
-      </c>
-      <c r="E283" s="85" t="s">
-        <v>249</v>
-      </c>
-      <c r="F283" s="85" t="s">
-        <v>250</v>
-      </c>
-      <c r="G283" s="85" t="s">
-        <v>262</v>
-      </c>
-      <c r="H283" s="85" t="s">
-        <v>249</v>
-      </c>
-      <c r="I283" s="85" t="s">
-        <v>249</v>
-      </c>
-      <c r="J283" s="85" t="s">
-        <v>259</v>
-      </c>
-      <c r="K283" s="85" t="s">
-        <v>31</v>
-      </c>
-      <c r="L283" s="85" t="s">
-        <v>31</v>
-      </c>
-      <c r="M283" s="85" t="s">
-        <v>256</v>
-      </c>
-      <c r="N283" s="85" t="s">
-        <v>264</v>
-      </c>
-      <c r="O283" s="86" t="s">
-        <v>48</v>
-      </c>
-      <c r="P283" s="85" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q283" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="R283" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="S283" s="68">
-        <v>1825</v>
-      </c>
-      <c r="T283" s="65" t="s">
-        <v>25</v>
-      </c>
+      <c r="A283" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="B283" s="85"/>
+      <c r="C283" s="85"/>
+      <c r="D283" s="85"/>
+      <c r="E283" s="85"/>
+      <c r="F283" s="85"/>
+      <c r="G283" s="85"/>
+      <c r="H283" s="85"/>
+      <c r="I283" s="85"/>
+      <c r="J283" s="85"/>
+      <c r="K283" s="85"/>
+      <c r="L283" s="85"/>
+      <c r="M283" s="85"/>
+      <c r="N283" s="85"/>
+      <c r="O283" s="85"/>
+      <c r="P283" s="85"/>
+      <c r="Q283" s="85"/>
     </row>
     <row r="284" spans="1:22">
       <c r="A284" s="84">
-        <v>90123</v>
+        <v>90001</v>
       </c>
       <c r="B284" s="85" t="s">
         <v>260</v>
@@ -25764,7 +25913,7 @@
         <v>55</v>
       </c>
       <c r="D284" s="85" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E284" s="85" t="s">
         <v>249</v>
@@ -25794,7 +25943,7 @@
         <v>256</v>
       </c>
       <c r="N284" s="85" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="O284" s="86" t="s">
         <v>48</v>
@@ -25812,6 +25961,130 @@
         <v>1825</v>
       </c>
       <c r="T284" s="65" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="285" spans="1:22">
+      <c r="A285" s="84">
+        <v>90012</v>
+      </c>
+      <c r="B285" s="85" t="s">
+        <v>260</v>
+      </c>
+      <c r="C285" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="D285" s="85" t="s">
+        <v>254</v>
+      </c>
+      <c r="E285" s="85" t="s">
+        <v>249</v>
+      </c>
+      <c r="F285" s="85" t="s">
+        <v>250</v>
+      </c>
+      <c r="G285" s="85" t="s">
+        <v>262</v>
+      </c>
+      <c r="H285" s="85" t="s">
+        <v>249</v>
+      </c>
+      <c r="I285" s="85" t="s">
+        <v>249</v>
+      </c>
+      <c r="J285" s="85" t="s">
+        <v>259</v>
+      </c>
+      <c r="K285" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="L285" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="M285" s="85" t="s">
+        <v>256</v>
+      </c>
+      <c r="N285" s="85" t="s">
+        <v>264</v>
+      </c>
+      <c r="O285" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="P285" s="85" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q285" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="R285" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="S285" s="68">
+        <v>1825</v>
+      </c>
+      <c r="T285" s="65" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="286" spans="1:22">
+      <c r="A286" s="84">
+        <v>90123</v>
+      </c>
+      <c r="B286" s="85" t="s">
+        <v>260</v>
+      </c>
+      <c r="C286" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="D286" s="85" t="s">
+        <v>255</v>
+      </c>
+      <c r="E286" s="85" t="s">
+        <v>249</v>
+      </c>
+      <c r="F286" s="85" t="s">
+        <v>250</v>
+      </c>
+      <c r="G286" s="85" t="s">
+        <v>262</v>
+      </c>
+      <c r="H286" s="85" t="s">
+        <v>249</v>
+      </c>
+      <c r="I286" s="85" t="s">
+        <v>249</v>
+      </c>
+      <c r="J286" s="85" t="s">
+        <v>259</v>
+      </c>
+      <c r="K286" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="L286" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="M286" s="85" t="s">
+        <v>256</v>
+      </c>
+      <c r="N286" s="85" t="s">
+        <v>252</v>
+      </c>
+      <c r="O286" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="P286" s="85" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q286" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="R286" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="S286" s="68">
+        <v>1825</v>
+      </c>
+      <c r="T286" s="65" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>